<commit_message>
various new functions including time-discounting, new summary metrics (e.g. hospital demand) etc
</commit_message>
<xml_diff>
--- a/data/IFR Distributions.xlsx
+++ b/data/IFR Distributions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\CEPI\SARS-3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\CEPI\SARS-3\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05E2CFD-3017-41D7-8E0F-EB171BEE99E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955235BB-A399-43C4-9A42-356D73F073FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="17" yWindow="17" windowWidth="16440" windowHeight="10269" xr2:uid="{284B3D5D-A2BE-479B-98E1-6CE21B1FF816}"/>
+    <workbookView xWindow="171" yWindow="540" windowWidth="28655" windowHeight="16877" xr2:uid="{284B3D5D-A2BE-479B-98E1-6CE21B1FF816}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1570,14 +1570,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>649060</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1359</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>10205</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>440871</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>136072</xdr:rowOff>
     </xdr:to>
@@ -1896,7 +1896,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1907,21 +1907,21 @@
   <dimension ref="A1:T33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.4609375" customWidth="1"/>
-    <col min="4" max="4" width="13.15234375" customWidth="1"/>
-    <col min="5" max="5" width="14.07421875" customWidth="1"/>
-    <col min="6" max="7" width="14.4609375" customWidth="1"/>
-    <col min="9" max="9" width="11.84375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31.3046875" customWidth="1"/>
-    <col min="14" max="14" width="15.69140625" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="6" max="7" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.28515625" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2011,7 +2011,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2023,11 +2023,11 @@
         <v>1.1019999999999999E-3</v>
       </c>
       <c r="D3">
-        <f>C3*$O$2</f>
+        <f t="shared" ref="D2:D18" si="1">C3*$O$2</f>
         <v>5.5099999999999995E-4</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E18" si="1">F3*$O$4</f>
+        <f t="shared" ref="E3:E18" si="2">F3*$O$4</f>
         <v>1.5200000000000001E-3</v>
       </c>
       <c r="F3">
@@ -2037,11 +2037,11 @@
         <v>4119566</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I18" si="2">C3*(D3*F3+(1-D3)*E3)</f>
+        <f t="shared" ref="I3:I18" si="3">C3*(D3*F3+(1-D3)*E3)</f>
         <v>1.67642442056E-6</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J18" si="3">I3*H3</f>
+        <f t="shared" ref="J3:J18" si="4">I3*H3</f>
         <v>6.9061410445086766</v>
       </c>
       <c r="M3" t="s">
@@ -2063,7 +2063,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2075,11 +2075,11 @@
         <v>1.1019999999999999E-3</v>
       </c>
       <c r="D4">
-        <f>C4*$O$2</f>
+        <f t="shared" si="1"/>
         <v>5.5099999999999995E-4</v>
       </c>
       <c r="E4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.5200000000000001E-3</v>
       </c>
       <c r="F4">
@@ -2089,11 +2089,11 @@
         <v>3956340</v>
       </c>
       <c r="I4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.67642442056E-6</v>
       </c>
       <c r="J4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.6325049920383501</v>
       </c>
       <c r="M4" t="s">
@@ -2115,7 +2115,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2127,11 +2127,11 @@
         <v>1.1019999999999999E-3</v>
       </c>
       <c r="D5">
-        <f>C5*$O$2</f>
+        <f t="shared" si="1"/>
         <v>5.5099999999999995E-4</v>
       </c>
       <c r="E5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.5200000000000001E-3</v>
       </c>
       <c r="F5">
@@ -2141,15 +2141,15 @@
         <v>3686133</v>
       </c>
       <c r="I5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.67642442056E-6</v>
       </c>
       <c r="J5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.1795233786320942</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2161,11 +2161,11 @@
         <v>2.2039999999999998E-3</v>
       </c>
       <c r="D6">
-        <f>C6*$O$2</f>
+        <f t="shared" si="1"/>
         <v>1.1019999999999999E-3</v>
       </c>
       <c r="E6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.0400000000000002E-3</v>
       </c>
       <c r="F6">
@@ -2175,15 +2175,15 @@
         <v>4074640</v>
       </c>
       <c r="I6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.7112353644800002E-6</v>
       </c>
       <c r="J6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>27.345868065524787</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2195,11 +2195,11 @@
         <v>3.3059999999999999E-3</v>
       </c>
       <c r="D7">
-        <f>C7*$O$2</f>
+        <f t="shared" si="1"/>
         <v>1.653E-3</v>
       </c>
       <c r="E7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.5600000000000007E-3</v>
       </c>
       <c r="F7">
@@ -2209,15 +2209,15 @@
         <v>4484067</v>
       </c>
       <c r="I7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.511273935512E-5</v>
       </c>
       <c r="J7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>67.766535821894877</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2229,11 +2229,11 @@
         <v>4.4079999999999996E-3</v>
       </c>
       <c r="D8">
-        <f>C8*$O$2</f>
+        <f t="shared" si="1"/>
         <v>2.2039999999999998E-3</v>
       </c>
       <c r="E8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.0800000000000003E-3</v>
       </c>
       <c r="F8">
@@ -2243,15 +2243,15 @@
         <v>4706828</v>
       </c>
       <c r="I8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.688924291584E-5</v>
       </c>
       <c r="J8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>126.56304145507735</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2263,11 +2263,11 @@
         <v>6.6119999999999998E-3</v>
       </c>
       <c r="D9">
-        <f>C9*$O$2</f>
+        <f t="shared" si="1"/>
         <v>3.3059999999999999E-3</v>
       </c>
       <c r="E9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.1200000000000014E-3</v>
       </c>
       <c r="F9">
@@ -2277,15 +2277,15 @@
         <v>4588196</v>
       </c>
       <c r="I9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.0600474840960012E-5</v>
       </c>
       <c r="J9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>278.04685626339335</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2297,11 +2297,11 @@
         <v>8.8159999999999992E-3</v>
       </c>
       <c r="D10">
-        <f>C10*$O$2</f>
+        <f t="shared" si="1"/>
         <v>4.4079999999999996E-3</v>
       </c>
       <c r="E10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.2160000000000001E-2</v>
       </c>
       <c r="F10">
@@ -2311,15 +2311,15 @@
         <v>4308130</v>
       </c>
       <c r="I10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0791138332672001E-4</v>
       </c>
       <c r="J10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>464.89626785134226</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2331,11 +2331,11 @@
         <v>1.1019999999999999E-2</v>
       </c>
       <c r="D11">
-        <f>C11*$O$2</f>
+        <f t="shared" si="1"/>
         <v>5.5099999999999993E-3</v>
       </c>
       <c r="E11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.52E-2</v>
       </c>
       <c r="F11">
@@ -2345,15 +2345,15 @@
         <v>4296121</v>
       </c>
       <c r="I11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.6888842055999998E-4</v>
       </c>
       <c r="J11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>725.56509022464763</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2365,11 +2365,11 @@
         <v>2.2039999999999997E-2</v>
       </c>
       <c r="D12">
-        <f>C12*$O$2</f>
+        <f t="shared" si="1"/>
         <v>1.1019999999999999E-2</v>
       </c>
       <c r="E12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.04E-2</v>
       </c>
       <c r="F12">
@@ -2379,15 +2379,15 @@
         <v>4634540</v>
       </c>
       <c r="I12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.8109136447999988E-4</v>
       </c>
       <c r="J12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3156.5451723371389</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2399,11 +2399,11 @@
         <v>4.4079999999999994E-2</v>
       </c>
       <c r="D13">
-        <f>C13*$O$2</f>
+        <f t="shared" si="1"/>
         <v>2.2039999999999997E-2</v>
       </c>
       <c r="E13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.08E-2</v>
       </c>
       <c r="F13">
@@ -2413,15 +2413,15 @@
         <v>4538925</v>
       </c>
       <c r="I13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.7686669158400001E-3</v>
       </c>
       <c r="J13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12566.771480979072</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2433,11 +2433,11 @@
         <v>6.6119999999999984E-2</v>
       </c>
       <c r="D14">
-        <f>C14*$O$2</f>
+        <f t="shared" si="1"/>
         <v>3.3059999999999992E-2</v>
       </c>
       <c r="E14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.1200000000000003E-2</v>
       </c>
       <c r="F14">
@@ -2447,15 +2447,15 @@
         <v>3905016</v>
       </c>
       <c r="I14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.3291788409599991E-3</v>
       </c>
       <c r="J14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24715.544640810251</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2467,11 +2467,11 @@
         <v>8.8159999999999988E-2</v>
       </c>
       <c r="D15">
-        <f>C15*$O$2</f>
+        <f t="shared" si="1"/>
         <v>4.4079999999999994E-2</v>
       </c>
       <c r="E15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.1216</v>
       </c>
       <c r="F15">
@@ -2481,15 +2481,15 @@
         <v>3381761</v>
       </c>
       <c r="I15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.1429079326719997E-2</v>
       </c>
       <c r="J15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>38650.414733007943</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2501,11 +2501,11 @@
         <v>0.11019999999999999</v>
       </c>
       <c r="D16">
-        <f>C16*$O$2</f>
+        <f t="shared" si="1"/>
         <v>5.5099999999999996E-2</v>
       </c>
       <c r="E16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.15200000000000002</v>
       </c>
       <c r="F16">
@@ -2515,15 +2515,15 @@
         <v>3388488</v>
       </c>
       <c r="I16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.8134820560000001E-2</v>
       </c>
       <c r="J16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>61449.62184971328</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2535,11 +2535,11 @@
         <v>0.16529999999999997</v>
       </c>
       <c r="D17">
-        <f>C17*$O$2</f>
+        <f t="shared" si="1"/>
         <v>8.2649999999999987E-2</v>
       </c>
       <c r="E17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.22799999999999998</v>
       </c>
       <c r="F17">
@@ -2549,15 +2549,15 @@
         <v>2442147</v>
       </c>
       <c r="I17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.2360819389999985E-2</v>
       </c>
       <c r="J17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>103451.3479908303</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2569,11 +2569,11 @@
         <v>0.27549999999999997</v>
       </c>
       <c r="D18">
-        <f>C18*$O$2</f>
+        <f t="shared" si="1"/>
         <v>0.13774999999999998</v>
       </c>
       <c r="E18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.38</v>
       </c>
       <c r="F18">
@@ -2583,15 +2583,15 @@
         <v>3450616</v>
       </c>
       <c r="I18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.12632157124999996</v>
       </c>
       <c r="J18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>435887.23490038986</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H20">
         <f>SUM(H2:H18)</f>
         <v>67886004</v>
@@ -2601,12 +2601,12 @@
         <v>1.004027224386398E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.4">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" s="1"/>
     </row>
   </sheetData>

</xml_diff>